<commit_message>
Correção da tabela e adição de iterações
</commit_message>
<xml_diff>
--- a/tabela-resultados.xlsx
+++ b/tabela-resultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizd\Desktop\fafa e eu\5-exercicio-inicial-sobre-programacao-dinamica-rafael-c-e-luiz-e\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719A2BC5-8F9C-40B4-AE0A-71C8C4055654}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E3D6F8-C91C-4CD9-92D6-4E6EB4777E3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{1EAF10C1-5E8A-4C2A-AE2C-C2771CE7881E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>Ex - 1 ------------------------</t>
   </si>
@@ -241,17 +241,129 @@
     <t>não testado</t>
   </si>
   <si>
-    <t>Saída:</t>
-  </si>
-  <si>
     <t>Iterações</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Iterações </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(vetor A)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Iterações </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(vetor B)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Iterações </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(vetor C)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Iterações </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(vetor D)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Iterações </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(vetor E)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Iterações </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(vetor F)</t>
+    </r>
+  </si>
+  <si>
+    <t>Saída</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Iterações </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(vetor G)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,8 +387,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,24 +423,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -367,31 +481,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -436,25 +530,34 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -771,25 +874,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA94F305-09BC-4D90-9659-5FD615F21353}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" customWidth="1"/>
+    <col min="13" max="13" width="24.85546875" customWidth="1"/>
+    <col min="14" max="14" width="26.140625" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -799,153 +909,241 @@
       <c r="G1" s="11"/>
       <c r="H1" s="13"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="I2" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="K2" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="M2" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="12"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O2" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="4">
         <v>3</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="21">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5">
         <v>21</v>
       </c>
-      <c r="D3" s="5">
+      <c r="E3" s="21">
+        <v>67</v>
+      </c>
+      <c r="F3" s="5">
         <v>987</v>
       </c>
-      <c r="E3" s="5">
+      <c r="G3" s="21">
+        <v>3193</v>
+      </c>
+      <c r="H3" s="5">
         <v>2178309</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="I3" s="22">
+        <v>7049155</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="K3" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="L3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="11"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M3" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="6">
         <v>3</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="21">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7">
         <v>21</v>
       </c>
-      <c r="D4" s="7">
+      <c r="E4" s="21">
+        <v>8</v>
+      </c>
+      <c r="F4" s="7">
         <v>987</v>
       </c>
-      <c r="E4" s="7">
+      <c r="G4" s="21">
+        <v>16</v>
+      </c>
+      <c r="H4" s="7">
         <v>2178309</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="I4" s="22">
+        <v>32</v>
+      </c>
+      <c r="J4" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="K4" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="L4" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="11"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M4" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="5">
         <v>3</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="24">
+        <v>13</v>
+      </c>
+      <c r="D5" s="14">
         <v>21</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="21">
+        <v>25</v>
+      </c>
+      <c r="F5" s="5">
         <v>987</v>
       </c>
-      <c r="E5" s="4">
+      <c r="G5" s="21">
+        <v>49</v>
+      </c>
+      <c r="H5" s="5">
         <v>2178309</v>
       </c>
-      <c r="F5" s="4">
+      <c r="I5" s="21">
+        <v>97</v>
+      </c>
+      <c r="J5" s="5">
         <v>-1361106235</v>
       </c>
-      <c r="G5" s="4">
+      <c r="K5" s="21">
+        <v>775</v>
+      </c>
+      <c r="L5" s="5">
         <v>1556111435</v>
       </c>
-      <c r="H5" s="14">
+      <c r="M5" s="21">
+        <v>15267</v>
+      </c>
+      <c r="N5" s="14">
         <v>1242044891</v>
       </c>
-      <c r="I5" s="11"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="21">
-        <v>0</v>
-      </c>
-      <c r="C6" s="21">
-        <v>0</v>
-      </c>
-      <c r="D6" s="21">
-        <v>0</v>
-      </c>
-      <c r="E6" s="21">
-        <v>0</v>
-      </c>
-      <c r="F6" s="21">
-        <v>0</v>
-      </c>
-      <c r="G6" s="21">
-        <v>0</v>
-      </c>
-      <c r="H6" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="O5" s="24">
+        <v>164703</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+    </row>
+    <row r="7" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="17">
+      <c r="B9" s="25">
         <v>300</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E8" s="8"/>
+      <c r="C9" s="24">
+        <v>356</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>